<commit_message>
Gerando termos para DEV Alta Plataforma
</commit_message>
<xml_diff>
--- a/CARGOS_FILTRADOS.xlsx
+++ b/CARGOS_FILTRADOS.xlsx
@@ -271,16 +271,16 @@
     <t>colaborador95@outlook.com</t>
   </si>
   <si>
-    <t>SISFIN - SP</t>
-  </si>
-  <si>
-    <t>SIAPI</t>
-  </si>
-  <si>
-    <t>SIPEN</t>
-  </si>
-  <si>
-    <t>SISFIN - DF</t>
+    <t>SIGLA 5</t>
+  </si>
+  <si>
+    <t>SIGLA 1</t>
+  </si>
+  <si>
+    <t>SIGLA 2</t>
+  </si>
+  <si>
+    <t>SIGLA 4</t>
   </si>
   <si>
     <t>analista/desenvolvedor - alta plataforma</t>
@@ -694,10 +694,10 @@
         <v>29243</v>
       </c>
       <c r="C2">
-        <v>48194946080</v>
+        <v>99123456789</v>
       </c>
       <c r="D2">
-        <v>8630400</v>
+        <v>7392846</v>
       </c>
       <c r="E2" t="s">
         <v>46</v>
@@ -706,7 +706,7 @@
         <v>32403</v>
       </c>
       <c r="G2">
-        <v>33493360793</v>
+        <v>83920471562</v>
       </c>
       <c r="H2" t="s">
         <v>50</v>
@@ -729,10 +729,10 @@
         <v>24259</v>
       </c>
       <c r="C3">
-        <v>48737508899</v>
+        <v>98765432109</v>
       </c>
       <c r="D3">
-        <v>7949084</v>
+        <v>5918374</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
@@ -741,7 +741,7 @@
         <v>30205</v>
       </c>
       <c r="G3">
-        <v>45915006606</v>
+        <v>74829103647</v>
       </c>
       <c r="H3" t="s">
         <v>51</v>
@@ -764,10 +764,10 @@
         <v>23033</v>
       </c>
       <c r="C4">
-        <v>75327862923</v>
+        <v>93456789012</v>
       </c>
       <c r="D4">
-        <v>1075350</v>
+        <v>8203947</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -776,7 +776,7 @@
         <v>35711</v>
       </c>
       <c r="G4">
-        <v>37668984314</v>
+        <v>98374612058</v>
       </c>
       <c r="H4" t="s">
         <v>52</v>
@@ -799,10 +799,10 @@
         <v>24186</v>
       </c>
       <c r="C5">
-        <v>85945316180</v>
+        <v>94567890123</v>
       </c>
       <c r="D5">
-        <v>9795072</v>
+        <v>6739201</v>
       </c>
       <c r="E5" t="s">
         <v>46</v>
@@ -811,7 +811,7 @@
         <v>28436</v>
       </c>
       <c r="G5">
-        <v>44878846442</v>
+        <v>75938462019</v>
       </c>
       <c r="H5" t="s">
         <v>53</v>
@@ -834,10 +834,10 @@
         <v>23295</v>
       </c>
       <c r="C6">
-        <v>90954492477</v>
+        <v>94321098765</v>
       </c>
       <c r="D6">
-        <v>4923680</v>
+        <v>7029381</v>
       </c>
       <c r="E6" t="s">
         <v>48</v>
@@ -846,7 +846,7 @@
         <v>35241</v>
       </c>
       <c r="G6">
-        <v>17744105341</v>
+        <v>61092837456</v>
       </c>
       <c r="H6" t="s">
         <v>54</v>
@@ -869,10 +869,10 @@
         <v>34715</v>
       </c>
       <c r="C7">
-        <v>79698532368</v>
+        <v>98765432098</v>
       </c>
       <c r="D7">
-        <v>3625745</v>
+        <v>6482917</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -881,7 +881,7 @@
         <v>36830</v>
       </c>
       <c r="G7">
-        <v>65531070330</v>
+        <v>79482013647</v>
       </c>
       <c r="H7" t="s">
         <v>55</v>
@@ -904,10 +904,10 @@
         <v>32789</v>
       </c>
       <c r="C8">
-        <v>72563385852</v>
+        <v>94567892345</v>
       </c>
       <c r="D8">
-        <v>3288791</v>
+        <v>7193846</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -916,7 +916,7 @@
         <v>25844</v>
       </c>
       <c r="G8">
-        <v>11200265817</v>
+        <v>70293847156</v>
       </c>
       <c r="H8" t="s">
         <v>56</v>
@@ -939,10 +939,10 @@
         <v>34147</v>
       </c>
       <c r="C9">
-        <v>40608279118</v>
+        <v>92345679876</v>
       </c>
       <c r="D9">
-        <v>6997153</v>
+        <v>8039172</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
@@ -951,7 +951,7 @@
         <v>34976</v>
       </c>
       <c r="G9">
-        <v>11410371595</v>
+        <v>64829103647</v>
       </c>
       <c r="H9" t="s">
         <v>57</v>
@@ -974,10 +974,10 @@
         <v>33213</v>
       </c>
       <c r="C10">
-        <v>70271104816</v>
+        <v>96543219876</v>
       </c>
       <c r="D10">
-        <v>9277015</v>
+        <v>7659203</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -986,7 +986,7 @@
         <v>27951</v>
       </c>
       <c r="G10">
-        <v>21552438139</v>
+        <v>71938462019</v>
       </c>
       <c r="H10" t="s">
         <v>58</v>
@@ -1009,10 +1009,10 @@
         <v>26337</v>
       </c>
       <c r="C11">
-        <v>75637965313</v>
+        <v>95678431234</v>
       </c>
       <c r="D11">
-        <v>4362611</v>
+        <v>8491736</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
@@ -1021,7 +1021,7 @@
         <v>36639</v>
       </c>
       <c r="G11">
-        <v>45952700882</v>
+        <v>80391745612</v>
       </c>
       <c r="H11" t="s">
         <v>59</v>
@@ -1044,10 +1044,10 @@
         <v>34007</v>
       </c>
       <c r="C12">
-        <v>30021719597</v>
+        <v>94567893456</v>
       </c>
       <c r="D12">
-        <v>7851986</v>
+        <v>7291836</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
@@ -1056,7 +1056,7 @@
         <v>36151</v>
       </c>
       <c r="G12">
-        <v>97256715341</v>
+        <v>71092837456</v>
       </c>
       <c r="H12" t="s">
         <v>60</v>
@@ -1079,10 +1079,10 @@
         <v>29285</v>
       </c>
       <c r="C13">
-        <v>44488662153</v>
+        <v>92345678098</v>
       </c>
       <c r="D13">
-        <v>7703695</v>
+        <v>7902847</v>
       </c>
       <c r="E13" t="s">
         <v>49</v>
@@ -1091,7 +1091,7 @@
         <v>31783</v>
       </c>
       <c r="G13">
-        <v>71407390098</v>
+        <v>68492013647</v>
       </c>
       <c r="H13" t="s">
         <v>61</v>
@@ -1114,10 +1114,10 @@
         <v>23927</v>
       </c>
       <c r="C14">
-        <v>60867910572</v>
+        <v>96543218765</v>
       </c>
       <c r="D14">
-        <v>2797847</v>
+        <v>7819204</v>
       </c>
       <c r="E14" t="s">
         <v>48</v>
@@ -1126,7 +1126,7 @@
         <v>29500</v>
       </c>
       <c r="G14">
-        <v>90263704506</v>
+        <v>72918347156</v>
       </c>
       <c r="H14" t="s">
         <v>62</v>
@@ -1149,10 +1149,10 @@
         <v>28440</v>
       </c>
       <c r="C15">
-        <v>31079092204</v>
+        <v>95678430123</v>
       </c>
       <c r="D15">
-        <v>5014020</v>
+        <v>6038471</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -1161,7 +1161,7 @@
         <v>26924</v>
       </c>
       <c r="G15">
-        <v>19662789887</v>
+        <v>79028413647</v>
       </c>
       <c r="H15" t="s">
         <v>63</v>
@@ -1184,10 +1184,10 @@
         <v>29286</v>
       </c>
       <c r="C16">
-        <v>93377713265</v>
+        <v>98765430986</v>
       </c>
       <c r="D16">
-        <v>5912139</v>
+        <v>6891735</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
@@ -1196,7 +1196,7 @@
         <v>31377</v>
       </c>
       <c r="G16">
-        <v>33015001215</v>
+        <v>78192047156</v>
       </c>
       <c r="H16" t="s">
         <v>64</v>
@@ -1219,10 +1219,10 @@
         <v>25364</v>
       </c>
       <c r="C17">
-        <v>13917639772</v>
+        <v>92345677098</v>
       </c>
       <c r="D17">
-        <v>2275423</v>
+        <v>6203948</v>
       </c>
       <c r="E17" t="s">
         <v>49</v>
@@ -1231,7 +1231,7 @@
         <v>34233</v>
       </c>
       <c r="G17">
-        <v>30002217906</v>
+        <v>68917362019</v>
       </c>
       <c r="H17" t="s">
         <v>65</v>
@@ -1254,10 +1254,10 @@
         <v>35983</v>
       </c>
       <c r="C18">
-        <v>92051821486</v>
+        <v>96543217654</v>
       </c>
       <c r="D18">
-        <v>1817343</v>
+        <v>6309281</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
@@ -1266,7 +1266,7 @@
         <v>36746</v>
       </c>
       <c r="G18">
-        <v>92875833716</v>
+        <v>75829103647</v>
       </c>
       <c r="H18" t="s">
         <v>66</v>
@@ -1289,10 +1289,10 @@
         <v>29005</v>
       </c>
       <c r="C19">
-        <v>98089663655</v>
+        <v>95678429012</v>
       </c>
       <c r="D19">
-        <v>2989924</v>
+        <v>7593841</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
@@ -1301,7 +1301,7 @@
         <v>22109</v>
       </c>
       <c r="G19">
-        <v>15655895816</v>
+        <v>62039447156</v>
       </c>
       <c r="H19" t="s">
         <v>67</v>
@@ -1324,10 +1324,10 @@
         <v>22198</v>
       </c>
       <c r="C20">
-        <v>94886028716</v>
+        <v>94321095432</v>
       </c>
       <c r="D20">
-        <v>8370681</v>
+        <v>8129374</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -1336,7 +1336,7 @@
         <v>32420</v>
       </c>
       <c r="G20">
-        <v>75550721049</v>
+        <v>79928462019</v>
       </c>
       <c r="H20" t="s">
         <v>68</v>
@@ -1359,10 +1359,10 @@
         <v>27916</v>
       </c>
       <c r="C21">
-        <v>28303445953</v>
+        <v>96543216543</v>
       </c>
       <c r="D21">
-        <v>4897956</v>
+        <v>6891734</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -1371,7 +1371,7 @@
         <v>26634</v>
       </c>
       <c r="G21">
-        <v>57173111062</v>
+        <v>62938462019</v>
       </c>
       <c r="H21" t="s">
         <v>69</v>
@@ -1394,10 +1394,10 @@
         <v>35354</v>
       </c>
       <c r="C22">
-        <v>30637944062</v>
+        <v>95678428098</v>
       </c>
       <c r="D22">
-        <v>9871872</v>
+        <v>7938472</v>
       </c>
       <c r="E22" t="s">
         <v>49</v>
@@ -1406,7 +1406,7 @@
         <v>23857</v>
       </c>
       <c r="G22">
-        <v>56047243374</v>
+        <v>69582047156</v>
       </c>
       <c r="H22" t="s">
         <v>70</v>
@@ -1429,10 +1429,10 @@
         <v>29778</v>
       </c>
       <c r="C23">
-        <v>66480466049</v>
+        <v>93456785432</v>
       </c>
       <c r="D23">
-        <v>6149684</v>
+        <v>6829174</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
@@ -1441,7 +1441,7 @@
         <v>27559</v>
       </c>
       <c r="G23">
-        <v>62987935864</v>
+        <v>79384762019</v>
       </c>
       <c r="H23" t="s">
         <v>71</v>
@@ -1464,10 +1464,10 @@
         <v>27248</v>
       </c>
       <c r="C24">
-        <v>69026407529</v>
+        <v>97890128901</v>
       </c>
       <c r="D24">
-        <v>2891464</v>
+        <v>6739202</v>
       </c>
       <c r="E24" t="s">
         <v>49</v>
@@ -1476,7 +1476,7 @@
         <v>27659</v>
       </c>
       <c r="G24">
-        <v>15387107611</v>
+        <v>68291713647</v>
       </c>
       <c r="H24" t="s">
         <v>72</v>
@@ -1499,10 +1499,10 @@
         <v>24536</v>
       </c>
       <c r="C25">
-        <v>28312867507</v>
+        <v>96543215432</v>
       </c>
       <c r="D25">
-        <v>5965737</v>
+        <v>7593844</v>
       </c>
       <c r="E25" t="s">
         <v>49</v>
@@ -1511,7 +1511,7 @@
         <v>23177</v>
       </c>
       <c r="G25">
-        <v>58157695482</v>
+        <v>74829162019</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
@@ -1534,10 +1534,10 @@
         <v>22049</v>
       </c>
       <c r="C26">
-        <v>78432147560</v>
+        <v>94567897890</v>
       </c>
       <c r="D26">
-        <v>1433458</v>
+        <v>6482916</v>
       </c>
       <c r="E26" t="s">
         <v>47</v>
@@ -1546,7 +1546,7 @@
         <v>33790</v>
       </c>
       <c r="G26">
-        <v>49581483902</v>
+        <v>79482047155</v>
       </c>
       <c r="H26" t="s">
         <v>74</v>
@@ -1569,10 +1569,10 @@
         <v>34177</v>
       </c>
       <c r="C27">
-        <v>57915665377</v>
+        <v>92345674098</v>
       </c>
       <c r="D27">
-        <v>7521932</v>
+        <v>5839203</v>
       </c>
       <c r="E27" t="s">
         <v>48</v>
@@ -1581,7 +1581,7 @@
         <v>33979</v>
       </c>
       <c r="G27">
-        <v>58554051144</v>
+        <v>83917413647</v>
       </c>
       <c r="H27" t="s">
         <v>75</v>
@@ -1604,10 +1604,10 @@
         <v>35085</v>
       </c>
       <c r="C28">
-        <v>90450590323</v>
+        <v>96543214321</v>
       </c>
       <c r="D28">
-        <v>1068463</v>
+        <v>8039171</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -1616,7 +1616,7 @@
         <v>32011</v>
       </c>
       <c r="G28">
-        <v>72670844811</v>
+        <v>64829147156</v>
       </c>
       <c r="H28" t="s">
         <v>76</v>
@@ -1639,10 +1639,10 @@
         <v>33185</v>
       </c>
       <c r="C29">
-        <v>56151392715</v>
+        <v>94321089876</v>
       </c>
       <c r="D29">
-        <v>8239645</v>
+        <v>6891733</v>
       </c>
       <c r="E29" t="s">
         <v>49</v>
@@ -1651,7 +1651,7 @@
         <v>34953</v>
       </c>
       <c r="G29">
-        <v>27598149773</v>
+        <v>62938413647</v>
       </c>
       <c r="H29" t="s">
         <v>77</v>
@@ -1674,10 +1674,10 @@
         <v>35013</v>
       </c>
       <c r="C30">
-        <v>63384049551</v>
+        <v>98765423219</v>
       </c>
       <c r="D30">
-        <v>8294960</v>
+        <v>7938471</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
@@ -1686,7 +1686,7 @@
         <v>29398</v>
       </c>
       <c r="G30">
-        <v>24489713610</v>
+        <v>69582062019</v>
       </c>
       <c r="H30" t="s">
         <v>78</v>
@@ -1709,10 +1709,10 @@
         <v>24471</v>
       </c>
       <c r="C31">
-        <v>39205218007</v>
+        <v>94567891234</v>
       </c>
       <c r="D31">
-        <v>1815188</v>
+        <v>7593846</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
@@ -1721,7 +1721,7 @@
         <v>22758</v>
       </c>
       <c r="G31">
-        <v>15864883636</v>
+        <v>68917313647</v>
       </c>
       <c r="H31" t="s">
         <v>79</v>
@@ -1744,10 +1744,10 @@
         <v>28690</v>
       </c>
       <c r="C32">
-        <v>12316308270</v>
+        <v>92345670098</v>
       </c>
       <c r="D32">
-        <v>5154395</v>
+        <v>6829173</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
@@ -1756,7 +1756,7 @@
         <v>34736</v>
       </c>
       <c r="G32">
-        <v>77150033528</v>
+        <v>79384747156</v>
       </c>
       <c r="H32" t="s">
         <v>80</v>
@@ -1779,10 +1779,10 @@
         <v>32204</v>
       </c>
       <c r="C33">
-        <v>31893325269</v>
+        <v>97890133456</v>
       </c>
       <c r="D33">
-        <v>1925142</v>
+        <v>7482914</v>
       </c>
       <c r="E33" t="s">
         <v>49</v>
@@ -1791,7 +1791,7 @@
         <v>29022</v>
       </c>
       <c r="G33">
-        <v>72938967123</v>
+        <v>61092813647</v>
       </c>
       <c r="H33" t="s">
         <v>81</v>
@@ -1814,10 +1814,10 @@
         <v>31804</v>
       </c>
       <c r="C34">
-        <v>94332141836</v>
+        <v>94321088765</v>
       </c>
       <c r="D34">
-        <v>6750439</v>
+        <v>7593847</v>
       </c>
       <c r="E34" t="s">
         <v>48</v>
@@ -1826,7 +1826,7 @@
         <v>28120</v>
       </c>
       <c r="G34">
-        <v>82059380577</v>
+        <v>74829113647</v>
       </c>
       <c r="H34" t="s">
         <v>82</v>
@@ -1849,10 +1849,10 @@
         <v>26845</v>
       </c>
       <c r="C35">
-        <v>32920517033</v>
+        <v>94567892345</v>
       </c>
       <c r="D35">
-        <v>9664966</v>
+        <v>8391744</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
@@ -1861,7 +1861,7 @@
         <v>34909</v>
       </c>
       <c r="G35">
-        <v>38236923825</v>
+        <v>75938462016</v>
       </c>
       <c r="H35" t="s">
         <v>83</v>
@@ -1884,10 +1884,10 @@
         <v>30378</v>
       </c>
       <c r="C36">
-        <v>15639674704</v>
+        <v>92345669098</v>
       </c>
       <c r="D36">
-        <v>7887262</v>
+        <v>7029383</v>
       </c>
       <c r="E36" t="s">
         <v>47</v>
@@ -1896,7 +1896,7 @@
         <v>27357</v>
       </c>
       <c r="G36">
-        <v>40407925162</v>
+        <v>61092847155</v>
       </c>
       <c r="H36" t="s">
         <v>84</v>

</xml_diff>